<commit_message>
[DEV] CC Studies Update
[DEV] CC Studies Update includes revised Drum Defintions and Updated Cases for C1- C5 including an Adjusted C4 Configuration and a theoretical C5 case.
</commit_message>
<xml_diff>
--- a/snapReactors/reactor_models/Automated Serpent Models/CCVerifcation.xlsx
+++ b/snapReactors/reactor_models/Automated Serpent Models/CCVerifcation.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaacnaupaaguirre/Documents/GitHub/SNAP-REACTORS/snapReactors/reactor_models/Automated Serpent Models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/iaguirre6_gatech_edu/Documents/SNAP 2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49AC7F01-B239-ED4F-A2E1-BAF4D938EA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{C0576130-31F3-3F42-B151-59CE4202366F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{497341D4-0D2D-664C-B078-35EE518736BE}"/>
   <bookViews>
-    <workbookView xWindow="19980" yWindow="1660" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{6D7706C2-2A02-478A-8E15-9410D5158D14}"/>
+    <workbookView xWindow="10900" yWindow="3880" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{6D7706C2-2A02-478A-8E15-9410D5158D14}"/>
   </bookViews>
   <sheets>
     <sheet name="Fuel and Core Comp Verification" sheetId="7" r:id="rId1"/>
     <sheet name="Core Configurations" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="129">
   <si>
     <t>Material</t>
   </si>
@@ -114,21 +115,6 @@
     <t>void</t>
   </si>
   <si>
-    <t>bpDens</t>
-  </si>
-  <si>
-    <t>ceramic Vol</t>
-  </si>
-  <si>
-    <t>dbDens</t>
-  </si>
-  <si>
-    <t>bpMass</t>
-  </si>
-  <si>
-    <t>dbMass</t>
-  </si>
-  <si>
     <t xml:space="preserve">     reflMix     </t>
   </si>
   <si>
@@ -138,24 +124,6 @@
     <t xml:space="preserve">Ceramic </t>
   </si>
   <si>
-    <t>Eff dens</t>
-  </si>
-  <si>
-    <t>Tot mass</t>
-  </si>
-  <si>
-    <t>bpMassFrac</t>
-  </si>
-  <si>
-    <t>dbMassFrac</t>
-  </si>
-  <si>
-    <t>TotMassFrac</t>
-  </si>
-  <si>
-    <t>8..18733</t>
-  </si>
-  <si>
     <t>MT</t>
   </si>
   <si>
@@ -345,9 +313,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>No. 6</t>
-  </si>
-  <si>
     <t>Experimental Excess Reactivity (cents)</t>
   </si>
   <si>
@@ -420,34 +385,46 @@
     <t>Apothem Eq. Hex.(in)</t>
   </si>
   <si>
-    <t>Apothem Eq. Hex.(cm)</t>
-  </si>
-  <si>
-    <t>Thickness Eq. Hex (cm)</t>
-  </si>
-  <si>
-    <t>Thickness Eq. Hex (in)</t>
-  </si>
-  <si>
-    <t>Total Eq. Hex Reflector Thickness (in)</t>
-  </si>
-  <si>
-    <t>Void Correction Factor</t>
-  </si>
-  <si>
-    <t>Adjusted Apothem Eq. Hex.(cm)</t>
-  </si>
-  <si>
-    <t>Adjusted Apothem Eq. Hex(in)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Configuration</t>
   </si>
   <si>
-    <t>Adjusted Eq.Hex Thickness (cm)</t>
+    <t>S-Hex Eq. Hex.(in)</t>
+  </si>
+  <si>
+    <t>Adjusted Thickness Eq.Hex (in)</t>
+  </si>
+  <si>
+    <t>Adjusted Apothem Eq.Hex (in)</t>
+  </si>
+  <si>
+    <t>Adjusted Apothem Eq.Hex (cm)</t>
+  </si>
+  <si>
+    <t>C-4*</t>
+  </si>
+  <si>
+    <t>No. 6 @ 105 Degrees</t>
+  </si>
+  <si>
+    <t>No. 6 @ 90 Degrees</t>
+  </si>
+  <si>
+    <t>C-5*</t>
+  </si>
+  <si>
+    <t>Modeled Infinite Multiplication Factor</t>
+  </si>
+  <si>
+    <t>Modeled Probability of Non-Leakage</t>
+  </si>
+  <si>
+    <t>Modeled Reproduction Factor</t>
+  </si>
+  <si>
+    <t>Modeled Thermal Fuel Utilization Factor</t>
   </si>
 </sst>
 </file>
@@ -455,12 +432,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="175" formatCode="0.00000"/>
-    <numFmt numFmtId="176" formatCode="0.0000"/>
-    <numFmt numFmtId="180" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,16 +471,56 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -511,29 +528,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,29 +968,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD98D26-166B-3E40-8864-727ACAD5733F}">
-  <dimension ref="A3:S89"/>
+  <dimension ref="A3:S95"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="62" workbookViewId="0">
-      <selection activeCell="L93" sqref="L93"/>
+    <sheetView topLeftCell="A53" zoomScale="131" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.5" customWidth="1"/>
   </cols>
@@ -970,7 +1033,7 @@
         <v>0.01</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F4" s="3">
         <f>C13+C14</f>
@@ -1130,19 +1193,19 @@
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="F10" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="N10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="O10" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="Q10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="R10" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
@@ -1172,10 +1235,10 @@
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="Q11" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="R11">
         <v>0.56999999999999995</v>
@@ -1203,14 +1266,14 @@
         <v>11.7475</v>
       </c>
       <c r="N12" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="O12">
         <f>0.532</f>
         <v>0.53200000000000003</v>
       </c>
       <c r="Q12" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="R12">
         <v>9.25</v>
@@ -1224,7 +1287,7 @@
         <v>2571.9699999999998</v>
       </c>
       <c r="D13" s="6">
-        <f>C13/$C$20</f>
+        <f t="shared" ref="D13:D19" si="1">C13/$C$20</f>
         <v>0.17641225418256931</v>
       </c>
       <c r="G13">
@@ -1236,14 +1299,14 @@
         <v>11.43</v>
       </c>
       <c r="N13" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="O13">
         <f>14</f>
         <v>14</v>
       </c>
       <c r="Q13" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="R13">
         <v>9</v>
@@ -1257,7 +1320,7 @@
         <v>10759.7</v>
       </c>
       <c r="D14" s="6">
-        <f>C14/$C$20</f>
+        <f t="shared" si="1"/>
         <v>0.73801130313658059</v>
       </c>
       <c r="G14">
@@ -1269,17 +1332,17 @@
         <v>11.7475</v>
       </c>
       <c r="N14" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="O14">
         <f>65203.782/211</f>
         <v>309.02266350710897</v>
       </c>
       <c r="Q14" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="R14" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
@@ -1290,7 +1353,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="6">
-        <f>C15/$C$20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F15" t="s">
@@ -1319,14 +1382,14 @@
         <v>0.79</v>
       </c>
       <c r="N15" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="O15" s="3">
         <f>(Q29+Q30)*O14</f>
         <v>30.399625537383411</v>
       </c>
       <c r="Q15" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="R15">
         <v>14</v>
@@ -1340,7 +1403,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="6">
-        <f>C16/$C$20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F16" t="s">
@@ -1369,26 +1432,25 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="N16" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="O16" s="4">
         <f>Q29/(Q29+Q30)</f>
         <v>0.93139561538199589</v>
       </c>
-      <c r="Q16" s="12" t="s">
+      <c r="Q16" t="s">
         <v>13</v>
       </c>
-      <c r="R16" s="12"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C17" s="5">
         <v>178.90100000000001</v>
       </c>
       <c r="D17" s="6">
-        <f>C17/$C$20</f>
+        <f t="shared" si="1"/>
         <v>1.2270877454058887E-2</v>
       </c>
       <c r="F17" t="s">
@@ -1417,13 +1479,13 @@
         <v>0.01</v>
       </c>
       <c r="N17" t="s">
+        <v>57</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q17" t="s">
         <v>68</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>79</v>
       </c>
       <c r="R17" s="2">
         <f>J15</f>
@@ -1438,7 +1500,7 @@
         <v>131.03100000000001</v>
       </c>
       <c r="D18" s="6">
-        <f>C18/$C$20</f>
+        <f t="shared" si="1"/>
         <v>8.9874586709006096E-3</v>
       </c>
       <c r="F18" t="s">
@@ -1467,14 +1529,14 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="N18" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="O18" s="4">
         <f>SUM(Q29:Q30)</f>
         <v>9.8373450000000001E-2</v>
       </c>
       <c r="Q18" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="R18">
         <f>L17</f>
@@ -1483,13 +1545,13 @@
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C19">
         <v>937.71400000000006</v>
       </c>
       <c r="D19" s="6">
-        <f>C19/$C$20</f>
+        <f t="shared" si="1"/>
         <v>6.4318106555890556E-2</v>
       </c>
       <c r="F19" t="s">
@@ -1518,7 +1580,7 @@
         <v>0.12</v>
       </c>
       <c r="N19" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="O19" s="4">
         <f>SUM(Q31:Q35)</f>
@@ -1549,7 +1611,7 @@
         <v>1.8152999999999999</v>
       </c>
       <c r="N20" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="O20" s="4">
         <f>SUM(Q27:Q28)</f>
@@ -1565,14 +1627,14 @@
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="N21" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="O21" s="3">
         <f>SUM(P27:P28)/SUM(P31:P35)</f>
         <v>1.6744988457024121</v>
       </c>
       <c r="Q21" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="R21" s="2">
         <f>J19</f>
@@ -1600,13 +1662,13 @@
         <v>0.79000924124987726</v>
       </c>
       <c r="N22" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="O22">
         <v>6.06</v>
       </c>
       <c r="Q22" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="R22" s="3">
         <f>O15*211/1000</f>
@@ -1634,7 +1696,7 @@
         <v>9.5324536408147986E-3</v>
       </c>
       <c r="Q23" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="R23" s="10">
         <f>F81</f>
@@ -1662,7 +1724,7 @@
         <v>1.3200465342089801E-2</v>
       </c>
       <c r="Q24" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="R24" s="10">
         <f>SUM(P27:P28)/P29</f>
@@ -1670,10 +1732,6 @@
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="E25">
-        <f>I24*35.56*G33</f>
-        <v>2.385928541903827</v>
-      </c>
       <c r="F25" t="s">
         <v>7</v>
       </c>
@@ -1693,19 +1751,15 @@
         <f>I25/$I$27</f>
         <v>6.8878051457132244E-2</v>
       </c>
-      <c r="N25" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
+      <c r="N25" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
       <c r="R25" s="4"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="E26">
-        <f>E25*211</f>
-        <v>503.43092234170751</v>
-      </c>
       <c r="F26" t="s">
         <v>24</v>
       </c>
@@ -1726,24 +1780,20 @@
         <v>0.11837978831008591</v>
       </c>
       <c r="N26" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="O26" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="P26" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="Q26" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="S26" s="1"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="D27">
-        <f>G34</f>
-        <v>4.03317535545024E-2</v>
-      </c>
       <c r="I27">
         <f>SUM(I22:I26)</f>
         <v>1.8152999999999999</v>
@@ -1762,10 +1812,6 @@
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="D28">
-        <f>E25</f>
-        <v>2.385928541903827</v>
-      </c>
       <c r="N28">
         <v>1002</v>
       </c>
@@ -1780,10 +1826,6 @@
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="D29">
-        <f>D27+D28</f>
-        <v>2.4262602954583294</v>
-      </c>
       <c r="N29">
         <v>92235</v>
       </c>
@@ -1798,10 +1840,6 @@
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="D30">
-        <f>D27/($D$29)</f>
-        <v>1.6623011813694782E-2</v>
-      </c>
       <c r="N30">
         <v>92238</v>
       </c>
@@ -1816,20 +1854,7 @@
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="D31">
-        <f>D28/($D$29)</f>
-        <v>0.98337698818630515</v>
-      </c>
-      <c r="F31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="5">
-        <v>2.3962805E-2</v>
-      </c>
-      <c r="H31">
-        <f>G31-0.005</f>
-        <v>1.8962804999999999E-2</v>
-      </c>
+      <c r="G31" s="5"/>
       <c r="N31">
         <v>40090</v>
       </c>
@@ -1844,12 +1869,6 @@
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="F32" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32">
-        <v>8.35</v>
-      </c>
       <c r="N32">
         <v>40091</v>
       </c>
@@ -1864,19 +1883,6 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F33" t="s">
-        <v>27</v>
-      </c>
-      <c r="G33">
-        <v>2.8</v>
-      </c>
-      <c r="J33">
-        <v>504.55159999999898</v>
-      </c>
-      <c r="K33" t="e">
-        <f>J33/$J$35</f>
-        <v>#VALUE!</v>
-      </c>
       <c r="N33">
         <v>40092</v>
       </c>
@@ -1891,19 +1897,6 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F34" t="s">
-        <v>28</v>
-      </c>
-      <c r="G34">
-        <v>4.03317535545024E-2</v>
-      </c>
-      <c r="J34" t="s">
-        <v>38</v>
-      </c>
-      <c r="K34" t="e">
-        <f>J34/$J$35</f>
-        <v>#VALUE!</v>
-      </c>
       <c r="N34">
         <v>40094</v>
       </c>
@@ -1918,17 +1911,6 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F35" t="s">
-        <v>29</v>
-      </c>
-      <c r="G35">
-        <f>G40*G33*((1/G39)-(G36/G32))</f>
-        <v>5.3571433646394405E-2</v>
-      </c>
-      <c r="J35" t="e">
-        <f>J33+J34</f>
-        <v>#VALUE!</v>
-      </c>
       <c r="N35">
         <v>40096</v>
       </c>
@@ -1943,13 +1925,6 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F36" t="s">
-        <v>35</v>
-      </c>
-      <c r="G36">
-        <f>G34/G40</f>
-        <v>4.03317535545024E-2</v>
-      </c>
       <c r="N36" t="s">
         <v>3</v>
       </c>
@@ -1963,45 +1938,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F37" t="s">
-        <v>36</v>
-      </c>
-      <c r="G37">
-        <f>G35/G40</f>
-        <v>5.3571433646394405E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F38" t="s">
-        <v>37</v>
-      </c>
-      <c r="G38">
-        <f>G37+G36</f>
-        <v>9.3903187200896798E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F39" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39">
-        <f>G40/G31</f>
-        <v>41.731341552042842</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F40" t="s">
-        <v>34</v>
-      </c>
-      <c r="G40">
-        <f>1</f>
-        <v>1</v>
-      </c>
-    </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B41">
         <v>517.42820626000002</v>
@@ -2009,7 +1948,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B42">
         <v>143.91228000000001</v>
@@ -2029,7 +1968,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B43">
         <v>146.91507999999999</v>
@@ -2049,7 +1988,7 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B44">
         <v>147.91466</v>
@@ -2069,7 +2008,7 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B45">
         <v>148.91728000000001</v>
@@ -2089,7 +2028,7 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B46">
         <v>149.91686000000001</v>
@@ -2109,7 +2048,7 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B47">
         <v>151.92008000000001</v>
@@ -2129,7 +2068,7 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B48">
         <v>153.92228</v>
@@ -2149,7 +2088,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E49" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F49" s="3">
         <f>SUM(F42:F48)</f>
@@ -2173,7 +2112,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E50" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F50" s="3">
         <f>B41*F49</f>
@@ -2190,7 +2129,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B51">
         <v>8.51</v>
@@ -2198,7 +2137,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B52">
         <v>143.91228000000001</v>
@@ -2218,7 +2157,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B53">
         <v>146.91507999999999</v>
@@ -2238,7 +2177,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B54">
         <v>147.91466</v>
@@ -2258,7 +2197,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B55">
         <v>148.91728000000001</v>
@@ -2278,7 +2217,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B56">
         <v>149.91686000000001</v>
@@ -2298,7 +2237,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B57">
         <v>151.92008000000001</v>
@@ -2318,7 +2257,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B58">
         <v>153.92228</v>
@@ -2338,7 +2277,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E59" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F59" s="3">
         <f>SUM(F52:F58)</f>
@@ -2347,7 +2286,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E60" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="F60" s="3">
         <v>0.13764000000000001</v>
@@ -2355,7 +2294,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E61" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F61" s="3">
         <f>B51*F59</f>
@@ -2364,7 +2303,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E62" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F62">
         <f>B51*F60</f>
@@ -2373,7 +2312,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E63" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F63" s="3">
         <f>F61+F62</f>
@@ -2382,7 +2321,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B65">
         <v>15.99492</v>
@@ -2402,7 +2341,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B68">
         <v>506.57964962</v>
@@ -2410,7 +2349,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B69">
         <v>143.91228000000001</v>
@@ -2430,7 +2369,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B70">
         <v>146.91507999999999</v>
@@ -2450,7 +2389,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B71">
         <v>147.91466</v>
@@ -2470,7 +2409,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B72">
         <v>148.91728000000001</v>
@@ -2490,7 +2429,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B73">
         <v>149.91686000000001</v>
@@ -2510,7 +2449,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B74">
         <v>151.92008000000001</v>
@@ -2530,7 +2469,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B75">
         <v>153.92228</v>
@@ -2550,7 +2489,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B76">
         <v>15.99492</v>
@@ -2570,7 +2509,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E77" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F77" s="3">
         <f>SUM(F69:F75)</f>
@@ -2579,7 +2518,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E78" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="F78" s="7">
         <f>0.137642*0.016799</f>
@@ -2588,7 +2527,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E79" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F79" s="3">
         <f>B68*F77</f>
@@ -2597,136 +2536,105 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E80" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="F80" s="3">
         <f>F78*B68</f>
         <v>1.1713377603982005</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E81" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F81" s="3">
         <f>F79+F80</f>
         <v>8.5100153021412464</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <f>B83*2.54</f>
+        <v>12.105640000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B83">
         <f>9.532/2</f>
         <v>4.766</v>
       </c>
       <c r="C83" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D83">
         <f>B83+F84</f>
         <v>4.8478000000000003</v>
       </c>
       <c r="E83" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F83">
         <v>12</v>
       </c>
-      <c r="G83">
-        <f>F83*2.54</f>
-        <v>30.48</v>
-      </c>
-      <c r="H83">
-        <f>G83/2</f>
-        <v>15.24</v>
-      </c>
-      <c r="I83" t="s">
-        <v>113</v>
-      </c>
-      <c r="J83">
-        <f>14.5</f>
-        <v>14.5</v>
-      </c>
-      <c r="K83">
-        <f>J83*2.54</f>
-        <v>36.83</v>
-      </c>
-      <c r="L83">
-        <f>K83/2</f>
-        <v>18.414999999999999</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B84">
         <f>14.5</f>
         <v>14.5</v>
       </c>
       <c r="C84" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D84">
         <v>4.68</v>
       </c>
       <c r="E84" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="F84">
         <f>0.0818</f>
         <v>8.1799999999999998E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
+        <v>106</v>
+      </c>
+      <c r="C85" t="s">
+        <v>108</v>
+      </c>
+      <c r="D85" t="s">
+        <v>112</v>
+      </c>
+      <c r="E85" t="s">
+        <v>109</v>
+      </c>
+      <c r="F85" t="s">
+        <v>113</v>
+      </c>
+      <c r="G85" t="s">
+        <v>117</v>
+      </c>
+      <c r="H85" t="s">
         <v>118</v>
       </c>
-      <c r="C85" t="s">
+      <c r="I85" t="s">
+        <v>119</v>
+      </c>
+      <c r="J85" t="s">
         <v>120</v>
       </c>
-      <c r="D85" t="s">
-        <v>124</v>
-      </c>
-      <c r="E85" t="s">
-        <v>121</v>
-      </c>
-      <c r="F85" t="s">
-        <v>125</v>
-      </c>
-      <c r="G85" t="s">
-        <v>126</v>
-      </c>
-      <c r="H85" t="s">
-        <v>127</v>
-      </c>
-      <c r="I85" t="s">
-        <v>131</v>
-      </c>
-      <c r="J85" t="s">
-        <v>129</v>
-      </c>
-      <c r="K85" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="L85" t="s">
-        <v>130</v>
-      </c>
-      <c r="M85" t="s">
-        <v>132</v>
-      </c>
-      <c r="N85" t="s">
-        <v>133</v>
-      </c>
-      <c r="O85" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M85" s="5"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B86">
         <v>2.34</v>
@@ -2748,44 +2656,25 @@
         <v>162.3087157593628</v>
       </c>
       <c r="G86">
-        <v>6.8449999999999998</v>
+        <f>SQRT(2*F86/(3*SQRT(3)))</f>
+        <v>7.9039644371454738</v>
       </c>
       <c r="H86">
-        <f>G86*2.54</f>
-        <v>17.386299999999999</v>
+        <f>(G86*SQRT(3)/2)-$D$83</f>
+        <v>1.997233993176752</v>
       </c>
       <c r="I86">
-        <f>1.01</f>
-        <v>1.01</v>
+        <f>1.005*G86*SQRT(3)/2</f>
+        <v>6.8792591631426356</v>
       </c>
       <c r="J86">
-        <f>$G$86-$D$83</f>
-        <v>1.9971999999999994</v>
-      </c>
-      <c r="K86">
-        <f>J86*2.54</f>
-        <v>5.072887999999999</v>
-      </c>
-      <c r="L86">
-        <f>J86</f>
-        <v>1.9971999999999994</v>
-      </c>
-      <c r="M86">
-        <f>I86*H86</f>
-        <v>17.560162999999999</v>
-      </c>
-      <c r="N86">
-        <f>M86/2.54</f>
-        <v>6.9134499999999992</v>
-      </c>
-      <c r="O86">
-        <f>M86-D83*2.54</f>
-        <v>5.2467509999999979</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+        <f>I86*2.54</f>
+        <v>17.473318274382294</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B87">
         <v>3.08</v>
@@ -2806,44 +2695,22 @@
         <f>F86+E87</f>
         <v>197.44913861616817</v>
       </c>
-      <c r="G87">
-        <v>7.55</v>
-      </c>
       <c r="H87">
-        <f t="shared" ref="H87:H89" si="1">G87*2.54</f>
-        <v>19.177</v>
+        <f>E87/6/$G$86</f>
+        <v>0.74098728421354909</v>
       </c>
       <c r="I87">
-        <v>1.0149999999999999</v>
+        <f>I86+H87</f>
+        <v>7.6202464473561848</v>
       </c>
       <c r="J87">
-        <f>G87-G86</f>
-        <v>0.70500000000000007</v>
-      </c>
-      <c r="K87">
-        <f t="shared" ref="K87:K89" si="2">J87*2.54</f>
-        <v>1.7907000000000002</v>
-      </c>
-      <c r="L87">
-        <f>L86+J87</f>
-        <v>2.7021999999999995</v>
-      </c>
-      <c r="M87">
-        <f t="shared" ref="M87:M89" si="3">I87*H87</f>
-        <v>19.464654999999997</v>
-      </c>
-      <c r="N87">
-        <f t="shared" ref="N87:N89" si="4">M87/2.54</f>
-        <v>7.6632499999999988</v>
-      </c>
-      <c r="O87">
-        <f>M87-M86</f>
-        <v>1.9044919999999976</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+        <f>I87*2.54</f>
+        <v>19.35542597628471</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B88">
         <v>3.78</v>
@@ -2853,56 +2720,33 @@
         <v>0.69999999999999973</v>
       </c>
       <c r="D88">
-        <f t="shared" ref="D88:D89" si="5">C88+D87</f>
+        <f t="shared" ref="D88:D89" si="2">C88+D87</f>
         <v>8.6278000000000006</v>
       </c>
       <c r="E88">
-        <f t="shared" ref="E88:E89" si="6">PI()*(D88^2 - D87^2)</f>
+        <f t="shared" ref="E88:E89" si="3">PI()*(D88^2 - D87^2)</f>
         <v>36.40766593503983</v>
       </c>
       <c r="F88">
-        <f t="shared" ref="F88:F89" si="7">F87+E88</f>
+        <f>F87+E88</f>
         <v>233.856804551208</v>
       </c>
-      <c r="G88">
-        <f>8.216</f>
-        <v>8.2159999999999993</v>
-      </c>
       <c r="H88">
-        <f t="shared" si="1"/>
-        <v>20.868639999999999</v>
+        <f>E88/6/$G$86</f>
+        <v>0.76770896058055693</v>
       </c>
       <c r="I88">
-        <v>1.0149999999999999</v>
+        <f t="shared" ref="I88:I89" si="4">I87+H88</f>
+        <v>8.387955407936742</v>
       </c>
       <c r="J88">
-        <f>G88-G87</f>
-        <v>0.66599999999999948</v>
-      </c>
-      <c r="K88">
-        <f t="shared" si="2"/>
-        <v>1.6916399999999987</v>
-      </c>
-      <c r="L88">
-        <f t="shared" ref="L88:L89" si="8">L87+J88</f>
-        <v>3.368199999999999</v>
-      </c>
-      <c r="M88">
-        <f t="shared" si="3"/>
-        <v>21.181669599999996</v>
-      </c>
-      <c r="N88">
-        <f t="shared" si="4"/>
-        <v>8.3392399999999984</v>
-      </c>
-      <c r="O88">
-        <f t="shared" ref="O88:O89" si="9">M88-M87</f>
-        <v>1.7170145999999988</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+        <f>I88*2.54</f>
+        <v>21.305406736159323</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B89">
         <v>4.7300000000000004</v>
@@ -2912,50 +2756,65 @@
         <v>0.95000000000000107</v>
       </c>
       <c r="D89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>9.5778000000000016</v>
       </c>
       <c r="E89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>54.334850253484674</v>
       </c>
       <c r="F89">
-        <f t="shared" si="7"/>
+        <f>F88+E89</f>
         <v>288.19165480469269</v>
       </c>
-      <c r="G89">
+      <c r="H89">
+        <f>E89/6/$G$86</f>
+        <v>1.1457298989127658</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="4"/>
+        <v>9.5336853068495078</v>
+      </c>
+      <c r="J89">
+        <f>I89*2.54</f>
+        <v>24.21556067939775</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M90" s="15"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G91" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C92">
+        <f>D83+D84</f>
+        <v>9.5277999999999992</v>
+      </c>
+      <c r="G92">
+        <v>6.8449999999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C93">
+        <f>C92*2.54</f>
+        <v>24.200612</v>
+      </c>
+      <c r="G93">
+        <v>7.55</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G94">
+        <f>8.216</f>
+        <v>8.2159999999999993</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G95">
         <v>9.1210000000000004</v>
-      </c>
-      <c r="H89">
-        <f t="shared" si="1"/>
-        <v>23.167340000000003</v>
-      </c>
-      <c r="I89">
-        <v>1.03</v>
-      </c>
-      <c r="J89">
-        <f>G89-G88</f>
-        <v>0.90500000000000114</v>
-      </c>
-      <c r="K89">
-        <f t="shared" si="2"/>
-        <v>2.2987000000000029</v>
-      </c>
-      <c r="L89">
-        <f t="shared" si="8"/>
-        <v>4.2732000000000001</v>
-      </c>
-      <c r="M89">
-        <f t="shared" si="3"/>
-        <v>23.862360200000005</v>
-      </c>
-      <c r="N89">
-        <f t="shared" si="4"/>
-        <v>9.3946300000000011</v>
-      </c>
-      <c r="O89">
-        <f t="shared" si="9"/>
-        <v>2.680690600000009</v>
       </c>
     </row>
   </sheetData>
@@ -2966,6 +2825,7 @@
     <mergeCell ref="N25:Q25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
@@ -2975,77 +2835,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C30F9B2-B5B9-A34F-84DE-0061747B4A1F}">
-  <dimension ref="A3:E18"/>
+  <dimension ref="A3:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="159" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="159" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
         <v>88</v>
       </c>
-      <c r="B4" t="s">
-        <v>99</v>
-      </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
         <v>90</v>
       </c>
-      <c r="B6" t="s">
-        <v>101</v>
-      </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B7">
         <v>38</v>
@@ -3062,7 +2924,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B8">
         <v>178</v>
@@ -3079,7 +2941,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B9">
         <v>9.6999999999999993</v>
@@ -3096,24 +2958,24 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="14">
+        <v>82</v>
+      </c>
+      <c r="B10" s="12">
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="12">
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="12">
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="12">
         <v>7.7000000000000002E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B11">
         <f>0.01*B9*$B$10*100000</f>
@@ -3134,7 +2996,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B12" s="6">
         <f>1+B11*0.00001</f>
@@ -3155,7 +3017,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -3166,30 +3028,30 @@
       <c r="D13">
         <v>1.5</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>105</v>
+      <c r="E13" s="11" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B15">
         <v>1.0008300000000001</v>
@@ -3203,7 +3065,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B16">
         <f>100000*(B15-1)/B15</f>
@@ -3218,9 +3080,9 @@
         <v>-147.21640811993342</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B17">
         <f>B16-B11</f>
@@ -3235,13 +3097,430 @@
         <v>68.383591880066604</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>134</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25">
+        <v>38</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25">
+        <v>21</v>
+      </c>
+      <c r="G25" s="5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="14">
+        <v>178</v>
+      </c>
+      <c r="C26" s="14">
+        <v>186</v>
+      </c>
+      <c r="D26" s="14">
+        <v>211</v>
+      </c>
+      <c r="E26" s="14">
+        <v>191</v>
+      </c>
+      <c r="F26" s="14">
+        <v>191</v>
+      </c>
+      <c r="G26" s="19">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C27">
+        <v>14.4</v>
+      </c>
+      <c r="D27">
+        <v>-28</v>
+      </c>
+      <c r="E27">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F27">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G27" s="5">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="16">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="C28" s="16">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="D28" s="16">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="E28" s="16">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="F28" s="16">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="G28" s="20">
+        <v>7.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29">
+        <f>0.01*B27*$B$10*100000</f>
+        <v>74.689999999999984</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:E29" si="2">0.01*C27*$B$10*100000</f>
+        <v>110.88000000000001</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>-215.60000000000002</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>71.610000000000014</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ref="F29" si="3">0.01*F27*$B$10*100000</f>
+        <v>71.610000000000014</v>
+      </c>
+      <c r="G29">
+        <f>0.01*G27*$B$10*100000</f>
+        <v>2879.8000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="17">
+        <f>1+B29*0.00001</f>
+        <v>1.0007469</v>
+      </c>
+      <c r="C30" s="17">
+        <f t="shared" ref="C30:E30" si="4">1+C29*0.00001</f>
+        <v>1.0011087999999999</v>
+      </c>
+      <c r="D30" s="17">
+        <f t="shared" si="4"/>
+        <v>0.99784399999999995</v>
+      </c>
+      <c r="E30" s="17">
+        <f t="shared" si="4"/>
+        <v>1.0007161</v>
+      </c>
+      <c r="F30" s="17">
+        <f t="shared" ref="F30" si="5">1+F29*0.00001</f>
+        <v>1.0007161</v>
+      </c>
+      <c r="G30" s="17">
+        <f>1+G29*0.00001</f>
+        <v>1.0287980000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31">
+        <v>1.00064</v>
+      </c>
+      <c r="C31">
+        <v>1.0016700000000001</v>
+      </c>
+      <c r="D31">
+        <f>0.99769</f>
+        <v>0.99768999999999997</v>
+      </c>
+      <c r="E31">
+        <v>0.99802999999999997</v>
+      </c>
+      <c r="F31">
+        <v>1.0003500000000001</v>
+      </c>
+      <c r="G31">
+        <v>1.02685</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="26">
+        <f t="shared" ref="B32:G32" si="6">100000*(B31-1)/B31</f>
+        <v>63.959066197630911</v>
+      </c>
+      <c r="C32" s="26">
+        <f t="shared" si="6"/>
+        <v>166.72157496980643</v>
+      </c>
+      <c r="D32" s="26">
+        <f t="shared" si="6"/>
+        <v>-231.53484549309246</v>
+      </c>
+      <c r="E32" s="26">
+        <f t="shared" si="6"/>
+        <v>-197.38885604641416</v>
+      </c>
+      <c r="F32" s="26">
+        <f t="shared" si="6"/>
+        <v>34.987754286007146</v>
+      </c>
+      <c r="G32" s="26">
+        <f t="shared" si="6"/>
+        <v>2614.7928129717134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="27">
+        <f t="shared" ref="B33:G33" si="7">ABS(B32-B29)</f>
+        <v>10.730933802369073</v>
+      </c>
+      <c r="C33" s="27">
+        <f t="shared" si="7"/>
+        <v>55.841574969806416</v>
+      </c>
+      <c r="D33" s="27">
+        <f t="shared" si="7"/>
+        <v>15.934845493092439</v>
+      </c>
+      <c r="E33" s="27">
+        <f t="shared" si="7"/>
+        <v>268.99885604641418</v>
+      </c>
+      <c r="F33" s="27">
+        <f t="shared" si="7"/>
+        <v>36.622245713992868</v>
+      </c>
+      <c r="G33" s="27">
+        <f t="shared" si="7"/>
+        <v>265.00718702828726</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="24">
+        <v>1.6390800000000001</v>
+      </c>
+      <c r="C34" s="24">
+        <v>1.6634</v>
+      </c>
+      <c r="D34" s="24">
+        <v>1.6850799999999999</v>
+      </c>
+      <c r="E34">
+        <v>1.6724600000000001</v>
+      </c>
+      <c r="F34" s="24">
+        <v>1.6724699999999999</v>
+      </c>
+      <c r="G34" s="6">
+        <v>1.6678999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+      <c r="A35" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="23">
+        <f>B31/B34</f>
+        <v>0.61048881079630035</v>
+      </c>
+      <c r="C35" s="23">
+        <f>C31/C34</f>
+        <v>0.60218227726343643</v>
+      </c>
+      <c r="D35" s="23">
+        <f>D31/D34</f>
+        <v>0.59207277992736251</v>
+      </c>
+      <c r="E35" s="23">
+        <f>E31/E34</f>
+        <v>0.59674371883333532</v>
+      </c>
+      <c r="F35" s="23">
+        <f>F31/F34</f>
+        <v>0.59812732066942909</v>
+      </c>
+      <c r="G35" s="23">
+        <f>G31/G34</f>
+        <v>0.61565441573235813</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" s="24">
+        <v>2.0011000000000001</v>
+      </c>
+      <c r="C36" s="24">
+        <v>2.0004</v>
+      </c>
+      <c r="D36" s="24">
+        <v>1.99919</v>
+      </c>
+      <c r="E36">
+        <v>2.0003299999999999</v>
+      </c>
+      <c r="F36" s="24">
+        <v>2.0003600000000001</v>
+      </c>
+      <c r="G36" s="24">
+        <v>2.0000300000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.25">
+      <c r="A37" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="22">
+        <v>0.86847799999999997</v>
+      </c>
+      <c r="C37" s="22">
+        <v>0.89410599999999996</v>
+      </c>
+      <c r="D37" s="22">
+        <v>0.92319099999999998</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.90189699999999995</v>
+      </c>
+      <c r="F37" s="22">
+        <v>0.90159900000000004</v>
+      </c>
+      <c r="G37" s="22">
+        <v>0.89528300000000005</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="B33:G33">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>